<commit_message>
Auto filtering data import penjualan, Ceo Hak akses
</commit_message>
<xml_diff>
--- a/public/csv/template_penjualan.xlsx
+++ b/public/csv/template_penjualan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agung\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40667E4B-387E-48F4-A05E-A3F642082C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0C45535-B01E-4CE7-90FA-02D28D1DEE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C42386B8-B996-4843-ABFF-B27F990450CB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>nama_konsumen</t>
   </si>
@@ -93,9 +93,6 @@
     <t>metode_pembayaran</t>
   </si>
   <si>
-    <t>PERCOBAAN IMPORT</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -106,6 +103,15 @@
   </si>
   <si>
     <t>pending</t>
+  </si>
+  <si>
+    <t>nik</t>
+  </si>
+  <si>
+    <t>Data 1</t>
+  </si>
+  <si>
+    <t>tgl_lahir</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5B4CDA-5082-4AE6-858E-0A6D5CA6A907}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,10 +489,11 @@
     <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,25 +551,31 @@
       <c r="S1" t="s">
         <v>9</v>
       </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>25</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -571,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="1">
         <v>45259</v>
@@ -591,6 +604,16 @@
       <c r="S2">
         <v>3</v>
       </c>
+      <c r="T2">
+        <v>123123123</v>
+      </c>
+      <c r="U2" s="1">
+        <v>36493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+      <c r="U3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>